<commit_message>
solved issue with loop reading coordinates
</commit_message>
<xml_diff>
--- a/Correct_excel.xlsx
+++ b/Correct_excel.xlsx
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,14 +395,6 @@
       </c>
       <c r="B3" s="1">
         <v>9.8618050000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>-83.363657000000003</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9.7618050000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved the unpack in Sexton function. Main script will now run and write to excel files
</commit_message>
<xml_diff>
--- a/Correct_excel.xlsx
+++ b/Correct_excel.xlsx
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +395,14 @@
       </c>
       <c r="B3" s="1">
         <v>9.8618050000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>-83.054317999999995</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.5982299999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a To DO LIST
UPdated excel sheet with test coordinates
</commit_message>
<xml_diff>
--- a/Correct_excel.xlsx
+++ b/Correct_excel.xlsx
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,25 +383,41 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>-83.629092</v>
+        <v>-83.31174</v>
       </c>
       <c r="B2" s="1">
-        <v>9.7039810000000006</v>
+        <v>9.0062099999999994</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>-84.363657000000003</v>
+        <v>-83.444000000000003</v>
       </c>
       <c r="B3" s="1">
-        <v>9.8618050000000004</v>
+        <v>9.8290000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>-83.629092</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9.7039810000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>-84.363657000000003</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.8618050000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>-83.054317999999995</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>8.5982299999999992</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added country codes and Chronosequence columns
</commit_message>
<xml_diff>
--- a/Correct_excel.xlsx
+++ b/Correct_excel.xlsx
@@ -16,12 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Chronosequence</t>
+  </si>
+  <si>
+    <t>CRI</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -361,63 +373,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
         <v>-83.31174</v>
       </c>
-      <c r="B2" s="1">
+      <c r="D2" s="1">
         <v>9.0062099999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
         <v>-83.444000000000003</v>
       </c>
-      <c r="B3" s="1">
+      <c r="D3" s="1">
         <v>9.8290000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
         <v>-83.629092</v>
       </c>
-      <c r="B4" s="1">
+      <c r="D4" s="1">
         <v>9.7039810000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
         <v>-84.363657000000003</v>
       </c>
-      <c r="B5" s="1">
+      <c r="D5" s="1">
         <v>9.8618050000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
         <v>-83.054317999999995</v>
       </c>
-      <c r="B6" s="1">
+      <c r="D6" s="1">
         <v>8.5982299999999992</v>
       </c>
     </row>

</xml_diff>